<commit_message>
update timeline & visio
</commit_message>
<xml_diff>
--- a/dokumentasi/timeline.xlsx
+++ b/dokumentasi/timeline.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>Plan</t>
   </si>
@@ -59,18 +59,6 @@
   </si>
   <si>
     <t>ACTIVITY</t>
-  </si>
-  <si>
-    <t>Activity 23</t>
-  </si>
-  <si>
-    <t>Activity 24</t>
-  </si>
-  <si>
-    <t>Activity 25</t>
-  </si>
-  <si>
-    <t>Activity 26</t>
   </si>
   <si>
     <r>
@@ -218,6 +206,45 @@
   </si>
   <si>
     <t>Retribusi &amp; barang</t>
+  </si>
+  <si>
+    <t>Retribusi : Revisi DB</t>
+  </si>
+  <si>
+    <t>Retribusi : Retribusi baru</t>
+  </si>
+  <si>
+    <t>Retribusi : Perbandingan Retribusi</t>
+  </si>
+  <si>
+    <t>Retribusi : Survey baru</t>
+  </si>
+  <si>
+    <t>Retribusi : Surat Penetapan Tarif</t>
+  </si>
+  <si>
+    <t>Retribusi : Surat perubahan tarif</t>
+  </si>
+  <si>
+    <t>Retribusi : Pencarian</t>
+  </si>
+  <si>
+    <t>Retirbusi : Rekap retribusi per periode</t>
+  </si>
+  <si>
+    <t>Retribusi : Rekap pelanggan PDAM</t>
+  </si>
+  <si>
+    <t>Retribusi : Rekap survey</t>
+  </si>
+  <si>
+    <t>Retribusi : Manage</t>
+  </si>
+  <si>
+    <t>Retribusi : Testing</t>
+  </si>
+  <si>
+    <t>Retribusi : Laporan survey baru</t>
   </si>
 </sst>
 </file>
@@ -492,11 +519,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -963,7 +990,7 @@
   <dimension ref="B2:BQ41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G4"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -978,24 +1005,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:69" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
+      <c r="B2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" spans="2:69" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
       <c r="I3" s="8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -1015,11 +1042,11 @@
       </c>
       <c r="X3" s="12"/>
       <c r="Y3" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AC3" s="13"/>
       <c r="AD3" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
@@ -1027,16 +1054,16 @@
       <c r="AJ3" s="1"/>
       <c r="AK3" s="14"/>
       <c r="AL3" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
       <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
@@ -1044,8 +1071,8 @@
       <c r="AX4" s="1"/>
     </row>
     <row r="5" spans="2:69" x14ac:dyDescent="0.3">
-      <c r="I5" s="21" t="s">
-        <v>36</v>
+      <c r="I5" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
@@ -1359,7 +1386,7 @@
     </row>
     <row r="9" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C9" s="16">
         <v>1</v>
@@ -1377,7 +1404,7 @@
     </row>
     <row r="10" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C10" s="16">
         <v>2</v>
@@ -1395,7 +1422,7 @@
     </row>
     <row r="11" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C11" s="16">
         <v>3</v>
@@ -1413,7 +1440,7 @@
     </row>
     <row r="12" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C12" s="16">
         <v>5</v>
@@ -1421,15 +1448,17 @@
       <c r="D12" s="16">
         <v>1</v>
       </c>
-      <c r="E12" s="16"/>
+      <c r="E12" s="16">
+        <v>6</v>
+      </c>
       <c r="F12" s="16"/>
       <c r="G12" s="17">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C13" s="16">
         <v>6</v>
@@ -1445,7 +1474,7 @@
     </row>
     <row r="14" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C14" s="16">
         <v>8</v>
@@ -1461,7 +1490,7 @@
     </row>
     <row r="15" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C15" s="16">
         <v>9</v>
@@ -1477,7 +1506,7 @@
     </row>
     <row r="16" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C16" s="16">
         <v>11</v>
@@ -1493,7 +1522,7 @@
     </row>
     <row r="17" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C17" s="16">
         <v>12</v>
@@ -1509,7 +1538,7 @@
     </row>
     <row r="18" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C18" s="16">
         <v>13</v>
@@ -1525,7 +1554,7 @@
     </row>
     <row r="19" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="15" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C19" s="16">
         <v>14</v>
@@ -1541,7 +1570,7 @@
     </row>
     <row r="20" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C20" s="18">
         <v>15</v>
@@ -1557,7 +1586,7 @@
     </row>
     <row r="21" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C21" s="18">
         <v>16</v>
@@ -1573,7 +1602,7 @@
     </row>
     <row r="22" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C22" s="16">
         <v>16</v>
@@ -1589,7 +1618,7 @@
     </row>
     <row r="23" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C23" s="16">
         <v>17</v>
@@ -1605,7 +1634,7 @@
     </row>
     <row r="24" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C24" s="16">
         <v>18</v>
@@ -1621,7 +1650,7 @@
     </row>
     <row r="25" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="15" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C25" s="16">
         <v>19</v>
@@ -1637,7 +1666,7 @@
     </row>
     <row r="26" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C26" s="16">
         <v>20</v>
@@ -1653,7 +1682,7 @@
     </row>
     <row r="27" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C27" s="16">
         <v>21</v>
@@ -1669,7 +1698,7 @@
     </row>
     <row r="28" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="15" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C28" s="16">
         <v>21</v>
@@ -1684,202 +1713,218 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C29" s="16">
         <v>21</v>
       </c>
       <c r="D29" s="16">
         <v>1</v>
       </c>
-      <c r="E29" s="16">
-        <v>12</v>
-      </c>
-      <c r="F29" s="16">
-        <v>5</v>
-      </c>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
       <c r="G29" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C30" s="16">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D30" s="16">
-        <v>5</v>
-      </c>
-      <c r="E30" s="16">
-        <v>14</v>
-      </c>
-      <c r="F30" s="16">
-        <v>6</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
       <c r="G30" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="C31" s="16">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D31" s="16">
-        <v>8</v>
-      </c>
-      <c r="E31" s="16">
-        <v>14</v>
-      </c>
-      <c r="F31" s="16">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
       <c r="G31" s="17">
-        <v>0.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="C32" s="16">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D32" s="16">
-        <v>7</v>
-      </c>
-      <c r="E32" s="16">
-        <v>14</v>
-      </c>
-      <c r="F32" s="16">
-        <v>3</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
       <c r="G32" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="15" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C33" s="16">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D33" s="16">
-        <v>4</v>
-      </c>
-      <c r="E33" s="16">
-        <v>15</v>
-      </c>
-      <c r="F33" s="16">
-        <v>8</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
       <c r="G33" s="17">
-        <v>0.12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="15" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="C34" s="16">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D34" s="16">
-        <v>5</v>
-      </c>
-      <c r="E34" s="16">
-        <v>15</v>
-      </c>
-      <c r="F34" s="16">
-        <v>3</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
       <c r="G34" s="17">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="15" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="C35" s="16">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D35" s="16">
-        <v>8</v>
-      </c>
-      <c r="E35" s="16">
-        <v>15</v>
-      </c>
-      <c r="F35" s="16">
-        <v>5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
       <c r="G35" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="15"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
+      <c r="B36" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="16">
+        <v>33</v>
+      </c>
+      <c r="D36" s="16">
+        <v>1</v>
+      </c>
       <c r="E36" s="16"/>
       <c r="F36" s="16"/>
-      <c r="G36" s="17"/>
+      <c r="G36" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="15"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
+      <c r="B37" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="16">
+        <v>34</v>
+      </c>
+      <c r="D37" s="16">
+        <v>1</v>
+      </c>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
-      <c r="G37" s="17"/>
+      <c r="G37" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="15"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
+      <c r="B38" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="16">
+        <v>35</v>
+      </c>
+      <c r="D38" s="16">
+        <v>1</v>
+      </c>
       <c r="E38" s="16"/>
       <c r="F38" s="16"/>
-      <c r="G38" s="17"/>
+      <c r="G38" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="15"/>
+      <c r="B39" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="C39" s="16">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D39" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" s="16"/>
       <c r="F39" s="16"/>
-      <c r="G39" s="17"/>
+      <c r="G39" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="15" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="C40" s="16">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="D40" s="16">
-        <v>28</v>
-      </c>
-      <c r="E40" s="16">
-        <v>16</v>
-      </c>
-      <c r="F40" s="16">
-        <v>30</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
       <c r="G40" s="17">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C41" s="1">
-        <v>17</v>
-      </c>
-      <c r="D41" s="1">
-        <v>2</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="16">
+        <v>38</v>
+      </c>
+      <c r="D41" s="16">
+        <v>1</v>
+      </c>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="17">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:G4"/>
   </mergeCells>
-  <conditionalFormatting sqref="I9:BP40">
+  <conditionalFormatting sqref="I9:BP41">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -1905,7 +1950,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B41:BP41">
+  <conditionalFormatting sqref="B42:BP42">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
add new project gudang
</commit_message>
<xml_diff>
--- a/dokumentasi/timeline.xlsx
+++ b/dokumentasi/timeline.xlsx
@@ -989,8 +989,8 @@
   </sheetPr>
   <dimension ref="B2:BQ41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1466,10 +1466,14 @@
       <c r="D13" s="16">
         <v>2</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
+      <c r="E13" s="16">
+        <v>9</v>
+      </c>
+      <c r="F13" s="16">
+        <v>1</v>
+      </c>
       <c r="G13" s="17">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>